<commit_message>
combined wordcount for multi volumes
</commit_message>
<xml_diff>
--- a/metadata-ELTEC-gsw.xlsx
+++ b/metadata-ELTEC-gsw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuliagrisot/Documents/GitHub/ELTeC-gsw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976C01BE-0C01-054C-AF41-BB3ACA31E73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640C6542-A640-2C41-BE83-CA76A85DF712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{75C0215C-EFA7-5044-9261-F41722653DFC}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$110</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="315">
   <si>
     <t>Author</t>
   </si>
@@ -975,6 +975,15 @@
   </si>
   <si>
     <t>GSW0135_zehender_leuenhof_1860.xml</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>second volume - same xml file: together word count = 121571, long</t>
+  </si>
+  <si>
+    <t>second volume - same xml file: together word count = 234406, long</t>
   </si>
 </sst>
 </file>
@@ -1084,20 +1093,9 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="9" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE6B3"/>
-          <bgColor rgb="FFFFE6B3"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color indexed="2"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1237,6 +1235,11 @@
           <bgColor rgb="FFFFE6B3"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="2"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1553,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD0BF6C-6DE1-F846-9053-7A31173332DF}">
-  <dimension ref="A1:N187"/>
+  <dimension ref="A1:O187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1578,7 +1581,7 @@
     <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1621,8 +1624,11 @@
       <c r="N1" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1713,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1836,7 +1842,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2003,7 +2009,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -2047,7 +2053,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>42</v>
       </c>
@@ -2346,7 +2352,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -2680,7 +2686,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>59</v>
       </c>
@@ -2721,7 +2727,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>61</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
@@ -2808,8 +2814,11 @@
       <c r="N29" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
@@ -2853,7 +2862,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>66</v>
       </c>
@@ -2897,7 +2906,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>66</v>
       </c>
@@ -3005,7 +3014,7 @@
         <v>1920</v>
       </c>
       <c r="H34" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(G34&lt;1949,"ja", IF(G34="please add","","nein"))</f>
         <v>ja</v>
       </c>
       <c r="I34" s="2" t="str">
@@ -5021,7 +5030,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>144</v>
       </c>
@@ -5062,7 +5071,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>144</v>
       </c>
@@ -5103,7 +5112,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>144</v>
       </c>
@@ -5144,7 +5153,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>148</v>
       </c>
@@ -5188,7 +5197,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>148</v>
       </c>
@@ -5232,7 +5241,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>148</v>
       </c>
@@ -5272,8 +5281,11 @@
       <c r="N86" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O86" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>148</v>
       </c>
@@ -5317,7 +5329,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>153</v>
       </c>
@@ -5358,7 +5370,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>153</v>
       </c>
@@ -5402,7 +5414,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>156</v>
       </c>
@@ -5443,7 +5455,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>156</v>
       </c>
@@ -5487,7 +5499,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>156</v>
       </c>
@@ -5528,7 +5540,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>156</v>
       </c>
@@ -5569,7 +5581,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>161</v>
       </c>
@@ -5613,7 +5625,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>161</v>
       </c>
@@ -5657,7 +5669,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>161</v>
       </c>
@@ -6550,111 +6562,117 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N110" xr:uid="{ABD0BF6C-6DE1-F846-9053-7A31173332DF}"/>
-  <conditionalFormatting sqref="A107:G110 A103:G103 A102:F102 A105:G105 A104:E104 A106:E106 M71:N71 M59:N59 M62:N63 M52:N54 M48:N49 M30:N30 M38:N45 M20:N27 L60:N61 L46:N47 L3:N19 L107:N107 L55:N58 L50:N51 L28:N29 L64:N70 L72:N98 A1:N2 A111:N1048576 L103:N103 H3:K110 A3:G101 L31:N37 L2:L110">
-    <cfRule type="containsText" dxfId="2" priority="34" operator="containsText" text="please add">
+  <conditionalFormatting sqref="A107:G110 A103:G103 A102:F102 A105:G105 A104:E104 A106:E106 M71:N71 M59:N59 M62:N63 M52:N54 M48:N49 M30:N30 M38:N45 M20:N27 L60:N61 L46:N47 L3:N19 L107:N107 L55:N58 L50:N51 L28:N29 L64:N70 L72:N98 A1:N2 A111:N1048576 L103:N103 H3:K110 A3:G101 L31:N37 L2:L110 O29">
+    <cfRule type="containsText" dxfId="22" priority="36" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="21" priority="35" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",#REF!)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L187">
-    <cfRule type="cellIs" dxfId="21" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
       <formula>"in progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H110">
-    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="nein">
+    <cfRule type="containsText" dxfId="19" priority="33" operator="containsText" text="nein">
       <formula>NOT(ISERROR(SEARCH("nein",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I280">
-    <cfRule type="containsText" dxfId="19" priority="30" operator="containsText" text="beyond">
+    <cfRule type="containsText" dxfId="18" priority="32" operator="containsText" text="beyond">
       <formula>NOT(ISERROR(SEARCH("beyond",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L187">
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="completed/in revision">
+    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="completed/in revision">
       <formula>NOT(ISERROR(SEARCH("completed/in revision",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C187">
-    <cfRule type="cellIs" dxfId="17" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="30" operator="greaterThan">
       <formula>1920</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L103">
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="29" operator="equal">
       <formula>"in progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F104:G104 F106:G106 N102 N108:N110 L99:N101 L104:N106">
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="14" priority="28" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",F99)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L103">
-    <cfRule type="containsText" dxfId="14" priority="24" operator="containsText" text="completed/in revision">
+    <cfRule type="containsText" dxfId="13" priority="26" operator="containsText" text="completed/in revision">
       <formula>NOT(ISERROR(SEARCH("completed/in revision",L103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102">
-    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",G102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L102">
-    <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",L102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L102">
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"in progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L102">
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="completed/in revision">
+    <cfRule type="containsText" dxfId="9" priority="19" operator="containsText" text="completed/in revision">
       <formula>NOT(ISERROR(SEARCH("completed/in revision",L102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L109">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",L109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L109">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"in progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L109">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="completed/in revision">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="completed/in revision">
       <formula>NOT(ISERROR(SEARCH("completed/in revision",L109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L110">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",L110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L110">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"in progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L110">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="completed/in revision">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="completed/in revision">
       <formula>NOT(ISERROR(SEARCH("completed/in revision",L110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M108:M110 M102">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="please add">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="please add">
       <formula>NOT(ISERROR(SEARCH("please add",M102)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O86">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="please add">
+      <formula>NOT(ISERROR(SEARCH("please add",O86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>